<commit_message>
Day 10 Part 1
</commit_message>
<xml_diff>
--- a/10/solve.xlsx
+++ b/10/solve.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rncole/PycharmProjects/adventofcode/10/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertcole/PycharmProjects/adventofcode/10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{393D3681-AE53-2F41-8CF4-2B746B8A6AF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EEE3DD-246B-A345-9452-0E7771F5EC1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{17248A8B-AA65-1F41-B1CF-4043F74C4DE4}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{17248A8B-AA65-1F41-B1CF-4043F74C4DE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Jolts</t>
   </si>
@@ -44,12 +44,18 @@
   <si>
     <t>3 count valid</t>
   </si>
+  <si>
+    <t>Lookup Values:</t>
+  </si>
+  <si>
+    <t>Part 2:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -62,6 +68,14 @@
       <color rgb="FF000000"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,11 +98,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,19 +426,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84FE7CC-59E8-C849-BC3C-9336FFCC304B}">
-  <dimension ref="A1:D104"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="G100" sqref="G100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="29.33203125" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,7 +449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -436,11 +459,15 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E2" t="str">
+        <f>IF(AND(D3="", D2 &lt;&gt; ""), VLOOKUP(D2,H$3:I$6, 2), "")</f>
+        <v/>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -453,15 +480,26 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D3:D6" si="0">IF(B3=1, IF(D2="",1,D2+1), "")</f>
+        <v>1</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E66" si="1">IF(AND(D4="", D3 &lt;&gt; ""), VLOOKUP(D3,H$3:I$6, 2), "")</f>
+        <v/>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B67" si="0">A4-A3</f>
+        <f t="shared" ref="B4:B67" si="2">A4-A3</f>
         <v>1</v>
       </c>
       <c r="C4">
@@ -469,15 +507,26 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C5">
@@ -485,32 +534,53 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>6</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C6">
         <f>IF(B6=3,IF(A6-A5&lt;=3,IF(A6-A4&lt;=3,IF(A6-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B6=3,IF(A7-A6&lt;=3,IF(A8-A6&lt;=3,IF(A9-A6&lt;=3,3,2),1),0),FALSE)</f>
         <v>2</v>
       </c>
-      <c r="D6">
-        <f>IF(C6&gt;0,C6-1,"")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>7</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C7">
@@ -518,32 +588,41 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f>IF(B7=1, IF(D6="",1,D6+1), "")</f>
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>10</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C8">
         <f>IF(B8=3,IF(A8-A7&lt;=3,IF(A8-A6&lt;=3,IF(A8-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B8=3,IF(A9-A8&lt;=3,IF(A10-A8&lt;=3,IF(A11-A8&lt;=3,3,2),1),0),FALSE)</f>
         <v>4</v>
       </c>
-      <c r="D8">
-        <f t="shared" ref="D7:D70" si="1">IF(C8&gt;0,C8-1,"")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D8" t="str">
+        <f t="shared" ref="D8:D71" si="3">IF(B8=1, IF(D7="",1,D7+1), "")</f>
+        <v/>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>11</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C9">
@@ -551,15 +630,20 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>12</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C10">
@@ -567,15 +651,20 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>13</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C11">
@@ -583,32 +672,41 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>16</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C12">
         <f>IF(B12=3,IF(A12-A11&lt;=3,IF(A12-A10&lt;=3,IF(A12-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B12=3,IF(A13-A12&lt;=3,IF(A14-A12&lt;=3,IF(A15-A12&lt;=3,3,2),1),0),FALSE)</f>
         <v>4</v>
       </c>
-      <c r="D12">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>17</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C13">
@@ -616,15 +714,20 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>18</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C14">
@@ -632,15 +735,20 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>19</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C15">
@@ -648,15 +756,20 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>20</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C16">
@@ -664,32 +777,41 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>23</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C17">
         <f>IF(B17=3,IF(A17-A16&lt;=3,IF(A17-A15&lt;=3,IF(A17-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B17=3,IF(A18-A17&lt;=3,IF(A19-A17&lt;=3,IF(A20-A17&lt;=3,3,2),1),0),FALSE)</f>
         <v>4</v>
       </c>
-      <c r="D17">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>24</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C18">
@@ -697,15 +819,20 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>25</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C19">
@@ -713,15 +840,20 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>26</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C20">
@@ -729,15 +861,20 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>27</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C21">
@@ -745,32 +882,41 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>30</v>
       </c>
       <c r="B22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C22">
         <f>IF(B22=3,IF(A22-A21&lt;=3,IF(A22-A20&lt;=3,IF(A22-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B22=3,IF(A23-A22&lt;=3,IF(A24-A22&lt;=3,IF(A25-A22&lt;=3,3,2),1),0),FALSE)</f>
         <v>4</v>
       </c>
-      <c r="D22">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D22" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>31</v>
       </c>
       <c r="B23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C23">
@@ -778,15 +924,20 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>32</v>
       </c>
       <c r="B24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C24">
@@ -794,15 +945,20 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>33</v>
       </c>
       <c r="B25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C25">
@@ -810,15 +966,20 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>34</v>
       </c>
       <c r="B26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C26">
@@ -826,32 +987,41 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>37</v>
       </c>
       <c r="B27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C27">
         <f>IF(B27=3,IF(A27-A26&lt;=3,IF(A27-A25&lt;=3,IF(A27-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B27=3,IF(A28-A27&lt;=3,IF(A29-A27&lt;=3,IF(A30-A27&lt;=3,3,2),1),0),FALSE)</f>
         <v>4</v>
       </c>
-      <c r="D27">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D27" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>38</v>
       </c>
       <c r="B28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C28">
@@ -859,15 +1029,20 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>39</v>
       </c>
       <c r="B29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C29">
@@ -875,15 +1050,20 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>40</v>
       </c>
       <c r="B30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C30">
@@ -891,15 +1071,20 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>41</v>
       </c>
       <c r="B31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C31">
@@ -907,83 +1092,104 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44</v>
       </c>
       <c r="B32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C32">
         <f>IF(B32=3,IF(A32-A31&lt;=3,IF(A32-A30&lt;=3,IF(A32-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B32=3,IF(A33-A32&lt;=3,IF(A34-A32&lt;=3,IF(A35-A32&lt;=3,3,2),1),0),FALSE)</f>
         <v>2</v>
       </c>
-      <c r="D32">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D32" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>47</v>
       </c>
       <c r="B33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C33">
         <f>IF(B33=3,IF(A33-A32&lt;=3,IF(A33-A31&lt;=3,IF(A33-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B33=3,IF(A34-A33&lt;=3,IF(A35-A33&lt;=3,IF(A36-A33&lt;=3,3,2),1),0),FALSE)</f>
         <v>2</v>
       </c>
-      <c r="D33">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D33" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>50</v>
       </c>
       <c r="B34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C34">
         <f>IF(B34=3,IF(A34-A33&lt;=3,IF(A34-A32&lt;=3,IF(A34-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B34=3,IF(A35-A34&lt;=3,IF(A36-A34&lt;=3,IF(A37-A34&lt;=3,3,2),1),0),FALSE)</f>
         <v>2</v>
       </c>
-      <c r="D34">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D34" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>53</v>
       </c>
       <c r="B35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C35">
         <f>IF(B35=3,IF(A35-A34&lt;=3,IF(A35-A33&lt;=3,IF(A35-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B35=3,IF(A36-A35&lt;=3,IF(A37-A35&lt;=3,IF(A38-A35&lt;=3,3,2),1),0),FALSE)</f>
         <v>3</v>
       </c>
-      <c r="D35">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D35" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>54</v>
       </c>
       <c r="B36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C36">
@@ -991,15 +1197,20 @@
         <v>0</v>
       </c>
       <c r="D36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>55</v>
       </c>
       <c r="B37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C37">
@@ -1007,49 +1218,62 @@
         <v>0</v>
       </c>
       <c r="D37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>58</v>
       </c>
       <c r="B38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C38">
         <f>IF(B38=3,IF(A38-A37&lt;=3,IF(A38-A36&lt;=3,IF(A38-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B38=3,IF(A39-A38&lt;=3,IF(A40-A38&lt;=3,IF(A41-A38&lt;=3,3,2),1),0),FALSE)</f>
         <v>2</v>
       </c>
-      <c r="D38">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D38" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>61</v>
       </c>
       <c r="B39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C39">
         <f>IF(B39=3,IF(A39-A38&lt;=3,IF(A39-A37&lt;=3,IF(A39-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B39=3,IF(A40-A39&lt;=3,IF(A41-A39&lt;=3,IF(A42-A39&lt;=3,3,2),1),0),FALSE)</f>
         <v>4</v>
       </c>
-      <c r="D39">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D39" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>62</v>
       </c>
       <c r="B40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C40">
@@ -1057,15 +1281,20 @@
         <v>0</v>
       </c>
       <c r="D40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>63</v>
       </c>
       <c r="B41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C41">
@@ -1073,15 +1302,20 @@
         <v>0</v>
       </c>
       <c r="D41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>64</v>
       </c>
       <c r="B42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C42">
@@ -1089,15 +1323,20 @@
         <v>0</v>
       </c>
       <c r="D42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>65</v>
       </c>
       <c r="B43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C43">
@@ -1105,32 +1344,41 @@
         <v>0</v>
       </c>
       <c r="D43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>68</v>
       </c>
       <c r="B44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C44">
         <f>IF(B44=3,IF(A44-A43&lt;=3,IF(A44-A42&lt;=3,IF(A44-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B44=3,IF(A45-A44&lt;=3,IF(A46-A44&lt;=3,IF(A47-A44&lt;=3,3,2),1),0),FALSE)</f>
         <v>4</v>
       </c>
-      <c r="D44">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D44" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>69</v>
       </c>
       <c r="B45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C45">
@@ -1138,15 +1386,20 @@
         <v>0</v>
       </c>
       <c r="D45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>70</v>
       </c>
       <c r="B46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C46">
@@ -1154,15 +1407,20 @@
         <v>0</v>
       </c>
       <c r="D46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>71</v>
       </c>
       <c r="B47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C47">
@@ -1170,15 +1428,20 @@
         <v>0</v>
       </c>
       <c r="D47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>72</v>
       </c>
       <c r="B48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C48">
@@ -1186,32 +1449,41 @@
         <v>0</v>
       </c>
       <c r="D48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>75</v>
       </c>
       <c r="B49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C49">
         <f>IF(B49=3,IF(A49-A48&lt;=3,IF(A49-A47&lt;=3,IF(A49-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B49=3,IF(A50-A49&lt;=3,IF(A51-A49&lt;=3,IF(A52-A49&lt;=3,3,2),1),0),FALSE)</f>
         <v>4</v>
       </c>
-      <c r="D49">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D49" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>76</v>
       </c>
       <c r="B50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C50">
@@ -1219,15 +1491,20 @@
         <v>0</v>
       </c>
       <c r="D50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>77</v>
       </c>
       <c r="B51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C51">
@@ -1235,15 +1512,20 @@
         <v>0</v>
       </c>
       <c r="D51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>78</v>
       </c>
       <c r="B52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C52">
@@ -1251,15 +1533,20 @@
         <v>0</v>
       </c>
       <c r="D52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>79</v>
       </c>
       <c r="B53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C53">
@@ -1267,32 +1554,41 @@
         <v>0</v>
       </c>
       <c r="D53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>82</v>
       </c>
       <c r="B54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C54">
         <f>IF(B54=3,IF(A54-A53&lt;=3,IF(A54-A52&lt;=3,IF(A54-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B54=3,IF(A55-A54&lt;=3,IF(A56-A54&lt;=3,IF(A57-A54&lt;=3,3,2),1),0),FALSE)</f>
         <v>2</v>
       </c>
-      <c r="D54">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D54" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>83</v>
       </c>
       <c r="B55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C55">
@@ -1300,49 +1596,62 @@
         <v>0</v>
       </c>
       <c r="D55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>86</v>
       </c>
       <c r="B56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C56">
         <f>IF(B56=3,IF(A56-A55&lt;=3,IF(A56-A54&lt;=3,IF(A56-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B56=3,IF(A57-A56&lt;=3,IF(A58-A56&lt;=3,IF(A59-A56&lt;=3,3,2),1),0),FALSE)</f>
         <v>2</v>
       </c>
-      <c r="D56">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D56" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>89</v>
       </c>
       <c r="B57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C57">
         <f>IF(B57=3,IF(A57-A56&lt;=3,IF(A57-A55&lt;=3,IF(A57-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B57=3,IF(A58-A57&lt;=3,IF(A59-A57&lt;=3,IF(A60-A57&lt;=3,3,2),1),0),FALSE)</f>
         <v>4</v>
       </c>
-      <c r="D57">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D57" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>90</v>
       </c>
       <c r="B58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C58">
@@ -1350,15 +1659,20 @@
         <v>0</v>
       </c>
       <c r="D58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>91</v>
       </c>
       <c r="B59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C59">
@@ -1366,15 +1680,20 @@
         <v>0</v>
       </c>
       <c r="D59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>92</v>
       </c>
       <c r="B60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C60">
@@ -1382,32 +1701,41 @@
         <v>0</v>
       </c>
       <c r="D60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>95</v>
       </c>
       <c r="B61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C61">
         <f>IF(B61=3,IF(A61-A60&lt;=3,IF(A61-A59&lt;=3,IF(A61-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B61=3,IF(A62-A61&lt;=3,IF(A63-A61&lt;=3,IF(A64-A61&lt;=3,3,2),1),0),FALSE)</f>
         <v>4</v>
       </c>
-      <c r="D61">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D61" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>96</v>
       </c>
       <c r="B62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C62">
@@ -1415,15 +1743,20 @@
         <v>0</v>
       </c>
       <c r="D62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>97</v>
       </c>
       <c r="B63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C63">
@@ -1431,15 +1764,20 @@
         <v>0</v>
       </c>
       <c r="D63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>98</v>
       </c>
       <c r="B64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C64">
@@ -1447,32 +1785,41 @@
         <v>0</v>
       </c>
       <c r="D64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>101</v>
       </c>
       <c r="B65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C65">
         <f>IF(B65=3,IF(A65-A64&lt;=3,IF(A65-A63&lt;=3,IF(A65-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B65=3,IF(A66-A65&lt;=3,IF(A67-A65&lt;=3,IF(A68-A65&lt;=3,3,2),1),0),FALSE)</f>
         <v>4</v>
       </c>
-      <c r="D65">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D65" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>102</v>
       </c>
       <c r="B66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C66">
@@ -1480,15 +1827,20 @@
         <v>0</v>
       </c>
       <c r="D66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E66" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>103</v>
       </c>
       <c r="B67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C67">
@@ -1496,15 +1848,20 @@
         <v>0</v>
       </c>
       <c r="D67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E67" t="str">
+        <f t="shared" ref="E67:E97" si="4">IF(AND(D68="", D67 &lt;&gt; ""), VLOOKUP(D67,H$3:I$6, 2), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>104</v>
       </c>
       <c r="B68">
-        <f t="shared" ref="B68:B96" si="2">A68-A67</f>
+        <f t="shared" ref="B68:B96" si="5">A68-A67</f>
         <v>1</v>
       </c>
       <c r="C68">
@@ -1512,15 +1869,20 @@
         <v>0</v>
       </c>
       <c r="D68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E68" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>105</v>
       </c>
       <c r="B69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C69">
@@ -1528,32 +1890,41 @@
         <v>0</v>
       </c>
       <c r="D69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>108</v>
       </c>
       <c r="B70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="C70">
         <f>IF(B70=3,IF(A70-A69&lt;=3,IF(A70-A68&lt;=3,IF(A70-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B70=3,IF(A71-A70&lt;=3,IF(A72-A70&lt;=3,IF(A73-A70&lt;=3,3,2),1),0),FALSE)</f>
         <v>4</v>
       </c>
-      <c r="D70">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D70" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E70" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>109</v>
       </c>
       <c r="B71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C71">
@@ -1561,15 +1932,20 @@
         <v>0</v>
       </c>
       <c r="D71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E71" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>110</v>
       </c>
       <c r="B72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C72">
@@ -1577,15 +1953,20 @@
         <v>0</v>
       </c>
       <c r="D72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D72:D97" si="6">IF(B72=1, IF(D71="",1,D71+1), "")</f>
+        <v>2</v>
+      </c>
+      <c r="E72" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>111</v>
       </c>
       <c r="B73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C73">
@@ -1593,15 +1974,20 @@
         <v>0</v>
       </c>
       <c r="D73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="E73" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>112</v>
       </c>
       <c r="B74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C74">
@@ -1609,32 +1995,41 @@
         <v>0</v>
       </c>
       <c r="D74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>115</v>
       </c>
       <c r="B75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="C75">
         <f>IF(B75=3,IF(A75-A74&lt;=3,IF(A75-A73&lt;=3,IF(A75-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B75=3,IF(A76-A75&lt;=3,IF(A77-A75&lt;=3,IF(A78-A75&lt;=3,3,2),1),0),FALSE)</f>
         <v>2</v>
       </c>
-      <c r="D75">
-        <f t="shared" ref="D71:D97" si="3">IF(C75&gt;0,C75-1,"")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D75" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E75" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>116</v>
       </c>
       <c r="B76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C76">
@@ -1642,31 +2037,41 @@
         <v>0</v>
       </c>
       <c r="D76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>119</v>
       </c>
       <c r="B77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="C77">
         <f>IF(B77=3,IF(A77-A76&lt;=3,IF(A77-A75&lt;=3,IF(A77-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B77=3,IF(A78-A77&lt;=3,IF(A79-A77&lt;=3,IF(A80-A77&lt;=3,3,2),1),0),FALSE)</f>
         <v>3</v>
       </c>
-      <c r="D77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D77" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E77" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>120</v>
       </c>
       <c r="B78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C78">
@@ -1674,15 +2079,20 @@
         <v>0</v>
       </c>
       <c r="D78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="E78" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>121</v>
       </c>
       <c r="B79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C79">
@@ -1690,32 +2100,41 @@
         <v>0</v>
       </c>
       <c r="D79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>124</v>
       </c>
       <c r="B80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="C80">
         <f>IF(B80=3,IF(A80-A79&lt;=3,IF(A80-A78&lt;=3,IF(A80-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B80=3,IF(A81-A80&lt;=3,IF(A82-A80&lt;=3,IF(A83-A80&lt;=3,3,2),1),0),FALSE)</f>
         <v>4</v>
       </c>
-      <c r="D80">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D80" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E80" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>125</v>
       </c>
       <c r="B81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C81">
@@ -1723,15 +2142,20 @@
         <v>0</v>
       </c>
       <c r="D81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="E81" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>126</v>
       </c>
       <c r="B82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C82">
@@ -1739,15 +2163,20 @@
         <v>0</v>
       </c>
       <c r="D82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="E82" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>127</v>
       </c>
       <c r="B83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C83">
@@ -1755,15 +2184,20 @@
         <v>0</v>
       </c>
       <c r="D83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="E83" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>128</v>
       </c>
       <c r="B84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C84">
@@ -1771,32 +2205,41 @@
         <v>0</v>
       </c>
       <c r="D84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>131</v>
       </c>
       <c r="B85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="C85">
         <f>IF(B85=3,IF(A85-A84&lt;=3,IF(A85-A83&lt;=3,IF(A85-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B85=3,IF(A86-A85&lt;=3,IF(A87-A85&lt;=3,IF(A88-A85&lt;=3,3,2),1),0),FALSE)</f>
         <v>4</v>
       </c>
-      <c r="D85">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D85" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E85" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>132</v>
       </c>
       <c r="B86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C86">
@@ -1804,15 +2247,20 @@
         <v>0</v>
       </c>
       <c r="D86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="E86" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>133</v>
       </c>
       <c r="B87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C87">
@@ -1820,15 +2268,20 @@
         <v>0</v>
       </c>
       <c r="D87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="E87" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>134</v>
       </c>
       <c r="B88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C88">
@@ -1836,15 +2289,20 @@
         <v>0</v>
       </c>
       <c r="D88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="E88" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>135</v>
       </c>
       <c r="B89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C89">
@@ -1852,49 +2310,62 @@
         <v>0</v>
       </c>
       <c r="D89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>138</v>
       </c>
       <c r="B90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="C90">
         <f>IF(B90=3,IF(A90-A89&lt;=3,IF(A90-A88&lt;=3,IF(A90-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B90=3,IF(A91-A90&lt;=3,IF(A92-A90&lt;=3,IF(A93-A90&lt;=3,3,2),1),0),FALSE)</f>
         <v>2</v>
       </c>
-      <c r="D90">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D90" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E90" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>141</v>
       </c>
       <c r="B91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="C91">
         <f>IF(B91=3,IF(A91-A90&lt;=3,IF(A91-A89&lt;=3,IF(A91-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B91=3,IF(A92-A91&lt;=3,IF(A93-A91&lt;=3,IF(A94-A91&lt;=3,3,2),1),0),FALSE)</f>
         <v>4</v>
       </c>
-      <c r="D91">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D91" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E91" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>142</v>
       </c>
       <c r="B92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C92">
@@ -1902,15 +2373,20 @@
         <v>0</v>
       </c>
       <c r="D92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="E92" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>143</v>
       </c>
       <c r="B93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C93">
@@ -1918,15 +2394,20 @@
         <v>0</v>
       </c>
       <c r="D93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="E93" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>144</v>
       </c>
       <c r="B94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C94">
@@ -1934,15 +2415,20 @@
         <v>0</v>
       </c>
       <c r="D94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="E94" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>145</v>
       </c>
       <c r="B95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="C95">
@@ -1950,25 +2436,35 @@
         <v>0</v>
       </c>
       <c r="D95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>148</v>
       </c>
       <c r="B96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="C96">
         <v>1</v>
       </c>
-      <c r="D96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="D96" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E96" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>151</v>
       </c>
@@ -1976,48 +2472,68 @@
         <f>IF(B97=3,IF(A97-A96&lt;=3,IF(A97-A95&lt;=3,IF(A97-#REF!&lt;=3,3,2),1),0),FALSE)+IF(B97=3,IF(A98-A97&lt;=3,IF(A99-A97&lt;=3,IF(A100-A97&lt;=3,3,2),1),0),FALSE)</f>
         <v>0</v>
       </c>
-      <c r="D97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D97" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E97" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C98" s="2"/>
-      <c r="D98" s="3">
-        <f>PRODUCT(D3:D97)</f>
-        <v>28697814</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>2</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="3">
         <f>COUNTIF(B2:B96,1)</f>
         <v>68</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C102" s="3"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>3</v>
       </c>
-      <c r="B103">
+      <c r="B103" s="3">
         <f>COUNTIF(B2:B96,3)+1</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>4</v>
-      </c>
-      <c r="B104">
+      <c r="C103" s="3"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B104" s="5">
         <f>B102*B103</f>
         <v>1904</v>
       </c>
+      <c r="C104" s="5"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B105" s="6">
+        <f>PRODUCT(E2:E97)</f>
+        <v>14173478093824</v>
+      </c>
+      <c r="C105" s="6"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A96">
     <sortCondition ref="A3:A96"/>
   </sortState>
+  <mergeCells count="4">
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B102:C102"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>